<commit_message>
Removed all Gear cards. Functionality of Gear cards are replaced by newly added skill cards. Changed skill cards cost.
</commit_message>
<xml_diff>
--- a/sheet/ChallengeCardData.xlsx
+++ b/sheet/ChallengeCardData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\datasheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F334482B-343F-4898-927D-C9BA8C947364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793717E6-F9BF-4C22-9E46-FCC5C2332DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,12 +110,6 @@
     <t>持续：房间宽度加1，高度加1，手牌基数在计算其他加成后翻倍。</t>
   </si>
   <si>
-    <t>挑战开始时：从额外牌堆将《收藏家》牌洗入主牌堆。&lt;br&gt;
-持续：横置的牌无法被正置。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《收藏家》牌放回额外牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>挑战开始时：重整。
 重整后：从额外牌堆向房间区所有列最前方发1张《沙虫》牌。&lt;br&gt;
 挑战结束时：将所有不在额外牌堆的《沙虫》牌放回额外牌堆。</t>
@@ -135,6 +129,12 @@
   <si>
     <t>挑战开始时：从额外牌堆选1张《红王》牌或1张《蓝王》牌洗入主牌堆。&lt;br&gt;
 挑战结束时：将所有不在额外牌堆的《红王》牌和《蓝王》牌放回额外牌堆。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑战开始时：从额外牌堆将《收藏家》牌洗入主牌堆。&lt;br&gt;
+持续：道具牌使用后横置。&lt;br&gt;
+挑战结束时：将所有道具牌正置，所有不在额外牌堆的《收藏家》牌放回额外牌堆。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,7 +466,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -546,7 +546,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -554,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
@@ -565,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="57" x14ac:dyDescent="0.2">
@@ -576,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -587,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed rules massively. Now player plays his cards into his own zone(namely player zone) and picks a row or column to starts a fight. He can start a fight at any time in the main phase. The monsters fight its opponent in the opposite zone(room zone vs player  zone). The resolution order of the fight is picked by the player, normally from left to right, up to down or vise versa. The cell in the room zone and player zone now has a name called slot. Certain abilities allow the player the start the battle with different slots other than slots in a row of a column. Also he can starts a battle with different resolution order if he has certain ability/item.
</commit_message>
<xml_diff>
--- a/sheet/ChallengeCardData.xlsx
+++ b/sheet/ChallengeCardData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793717E6-F9BF-4C22-9E46-FCC5C2332DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC74C06-4571-4865-ACED-45FE0A180224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>持续：房间宽度加1，高度加1，手牌基数在计算其他加成后翻倍。</t>
-  </si>
-  <si>
     <t>挑战开始时：重整。
 重整后：从额外牌堆向房间区所有列最前方发1张《沙虫》牌。&lt;br&gt;
 挑战结束时：将所有不在额外牌堆的《沙虫》牌放回额外牌堆。</t>
@@ -135,6 +132,10 @@
     <t>挑战开始时：从额外牌堆将《收藏家》牌洗入主牌堆。&lt;br&gt;
 持续：道具牌使用后横置。&lt;br&gt;
 挑战结束时：将所有道具牌正置，所有不在额外牌堆的《收藏家》牌放回额外牌堆。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>持续：房间宽度加1，高度加1，玩家重整时可以额外抽2张牌，翻选时可以额外翻2张牌、额外选1张牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,7 +467,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -510,7 +511,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
@@ -554,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
@@ -565,7 +566,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="57" x14ac:dyDescent="0.2">
@@ -576,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -587,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -598,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the effect of cursed coin and cursed Pot cards to make them stay longer in the player's Loot Zone. Added tag to item cards to indicate their archetype.
</commit_message>
<xml_diff>
--- a/sheet/ChallengeCardData.xlsx
+++ b/sheet/ChallengeCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC74C06-4571-4865-ACED-45FE0A180224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0422BFA6-1956-4AD4-A990-B416E4E72B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,38 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>持续：房间宽度固定为1，高度在计算其他加成后翻倍，手牌基数在计算其他加成后减半（向上取整）。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>持续：房间区最前方的牌在发牌时背面向上。&lt;br&gt;
-开战时：将战场中背面向上的牌翻正。&lt;br&gt;：
-回合结束时：选房间区1张牌翻正。</t>
-  </si>
-  <si>
-    <t>挑战开始时：重整。这之后，从额外牌堆将《命匣》牌洗入主牌堆。&lt;br&gt;
-重整后：从额外牌堆将《巫妖》牌放在房间区任意列最前方。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《巫妖》牌和《命匣》牌放回额外牌堆。</t>
-  </si>
-  <si>
-    <t>挑战开始时：重整。这之后，将主牌堆所有牌送墓，在此期间不触发任何效果。&lt;br&gt;
-重整后：从额外牌堆向房间区任意一列的最前方发1张《冠军》牌。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《冠军》牌放回额外牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>挑战开始时：重整。
-重整后：从额外牌堆向房间区所有列最前方发1张《沙虫》牌。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《沙虫》牌放回额外牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>挑战开始时：从额外牌堆将《时空吞噬者》牌洗入主牌堆。&lt;br&gt;
-持续：弃牌堆的牌无法移出弃牌堆，消耗时间时不弃牌，玩家不能休息。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《时空吞噬者》牌放回额外牌堆，然后将弃牌堆所有牌送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>挑战开始时：从额外牌堆将5张《手指》牌洗入主牌堆。&lt;br&gt;
 挑战结束时：将所有不在额外牌堆的《手指》牌放回额外牌堆。</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,7 +103,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>持续：房间宽度加1，高度加1，玩家重整时可以额外抽2张牌，翻选时可以额外翻2张牌、额外选1张牌。</t>
+    <t>房间区宽度降低至1，高度增加宽度降低的数值。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房间区中央的牌在发牌时背面向上。&lt;br&gt;
+开战时：将战场中背面向上的牌翻正。&lt;br&gt;
+回合结束时：选房间区1张牌翻正。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房间宽度加1，高度加1。&lt;br&gt;
+玩家手牌基数加3。&lt;br&gt;
+翻选时可以额外翻2张牌，额外选1张牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑战开始时：从额外牌堆将《命匣》牌洗入主牌堆。&lt;br&gt;
+重整后：从额外牌堆将1张《巫妖》牌放在房间区任意槽位中。&lt;br&gt;
+挑战结束时：将所有不在额外牌堆的《巫妖》牌和《命匣》牌放回额外牌堆。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑战开始时：将主牌堆所有牌送墓，此期间内牌的送墓时效果无效。&lt;br&gt;
+重整后：从额外牌堆将1张《冠军》牌放在房间区任意槽位中。&lt;br&gt;
+挑战结束时：将所有不在额外牌堆的《冠军》牌放回额外牌堆。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑战开始时：重整。
+重整后：从额外牌堆将2张《沙虫》牌分别放到房间区和备战区的任意槽位中。&lt;br&gt;
+挑战结束时：将所有不在额外牌堆的《沙虫》牌放回额外牌堆。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑战开始时：从额外牌堆将《时空吞噬者》牌洗入主牌堆。&lt;br&gt;
+持续：弃牌堆的牌无法移出弃牌堆，所有消耗时间的牌无效。&lt;br&gt;
+挑战结束时：将所有不在额外牌堆的《时空吞噬者》牌放回额外牌堆，然后将弃牌堆所有牌送墓。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -500,18 +504,18 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
@@ -522,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
@@ -533,10 +537,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -544,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="57" x14ac:dyDescent="0.2">
@@ -555,10 +559,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -566,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="57" x14ac:dyDescent="0.2">
@@ -577,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -588,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -599,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Misc card changes. Changed how challenge cards work. The player flip a Challenge card when the game starts. Every shuffle, an option on the challenge card is unlocked which adds to the difficulty.
</commit_message>
<xml_diff>
--- a/sheet/ChallengeCardData.xlsx
+++ b/sheet/ChallengeCardData.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0422BFA6-1956-4AD4-A990-B416E4E72B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9ADCE0-06AC-40E6-8DB7-D4891EE0265B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>cardName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,18 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>一线天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大房间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>迷雾</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>大墓地</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -71,75 +70,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>裂隙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>手层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>冲突层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>沙虫坑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>挑战开始时：从额外牌堆将5张《手指》牌洗入主牌堆。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《手指》牌放回额外牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>挑战开始时：从额外牌堆选1张《红王》牌或1张《蓝王》牌洗入主牌堆。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《红王》牌和《蓝王》牌放回额外牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>挑战开始时：从额外牌堆将《收藏家》牌洗入主牌堆。&lt;br&gt;
-持续：道具牌使用后横置。&lt;br&gt;
-挑战结束时：将所有道具牌正置，所有不在额外牌堆的《收藏家》牌放回额外牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>房间区宽度降低至1，高度增加宽度降低的数值。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>房间区中央的牌在发牌时背面向上。&lt;br&gt;
-开战时：将战场中背面向上的牌翻正。&lt;br&gt;
-回合结束时：选房间区1张牌翻正。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>房间宽度加1，高度加1。&lt;br&gt;
-玩家手牌基数加3。&lt;br&gt;
-翻选时可以额外翻2张牌，额外选1张牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>挑战开始时：从额外牌堆将《命匣》牌洗入主牌堆。&lt;br&gt;
-重整后：从额外牌堆将1张《巫妖》牌放在房间区任意槽位中。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《巫妖》牌和《命匣》牌放回额外牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>挑战开始时：将主牌堆所有牌送墓，此期间内牌的送墓时效果无效。&lt;br&gt;
-重整后：从额外牌堆将1张《冠军》牌放在房间区任意槽位中。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《冠军》牌放回额外牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>挑战开始时：重整。
-重整后：从额外牌堆将2张《沙虫》牌分别放到房间区和备战区的任意槽位中。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《沙虫》牌放回额外牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>挑战开始时：从额外牌堆将《时空吞噬者》牌洗入主牌堆。&lt;br&gt;
-持续：弃牌堆的牌无法移出弃牌堆，所有消耗时间的牌无效。&lt;br&gt;
-挑战结束时：将所有不在额外牌堆的《时空吞噬者》牌放回额外牌堆，然后将弃牌堆所有牌送墓。</t>
+    <t>DL2：房间尺寸加1。&lt;br&gt;
+DL3：房间尺寸加1。战斗中，战场外的牌无法移入战场，战场中的牌无法移出战场。&lt;br&gt;
+BOSS ：从额外牌堆将1张《冠军》牌放在房间区任意槽位中。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1。&lt;br&gt;
+DL3：房间尺寸加1。墓地中的牌不受玩家控制的牌的效果影响。&lt;br&gt;
+BOSS：从额外牌堆将1张《命匣》牌洗入主牌堆。每次重整后，从额外牌堆将《巫妖》牌放在房间区任意槽位中。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手指层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1。&lt;br&gt;
+DL3：房间尺寸加1。场上的牌无法移动到《沙虫》所在槽位中。&lt;br&gt;
+BOSS：从额外牌堆将3张《沙虫》牌依次放在房间区任意槽位中。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1。&lt;br&gt;
+DL3：房间尺寸加1。玩家的手牌只能被打出。&lt;br&gt;
+BOSS：从额外牌堆将5张《封印手指》牌洗入主牌堆。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷雾森林</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1。&lt;br&gt;
+DL3：房间尺寸加1。重整时，房间区中央的牌保持背面向上发出。&lt;br&gt;
+BOSS：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1。&lt;br&gt;
+DL3：房间尺寸加1。遗物牌使用后横置，且不会在回合结束时被复位。&lt;br&gt;
+BOSS：从额外牌堆将1张《收藏家》牌洗入主牌堆。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -468,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -496,18 +471,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -515,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
@@ -526,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
@@ -537,73 +512,29 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="57" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="57" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Massive update. But I cant remember what changes have been committed. I should make a double check list on what have been done and what have been committed.
</commit_message>
<xml_diff>
--- a/sheet/ChallengeCardData.xlsx
+++ b/sheet/ChallengeCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9ADCE0-06AC-40E6-8DB7-D4891EE0265B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E15CDEA-AFE6-48AC-AE22-A30A2580B04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,47 +74,45 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DL2：房间尺寸加1。&lt;br&gt;
-DL3：房间尺寸加1。战斗中，战场外的牌无法移入战场，战场中的牌无法移出战场。&lt;br&gt;
-BOSS ：从额外牌堆将1张《冠军》牌放在房间区任意槽位中。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DL2：房间尺寸加1。&lt;br&gt;
-DL3：房间尺寸加1。墓地中的牌不受玩家控制的牌的效果影响。&lt;br&gt;
-BOSS：从额外牌堆将1张《命匣》牌洗入主牌堆。每次重整后，从额外牌堆将《巫妖》牌放在房间区任意槽位中。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>手指层</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DL2：房间尺寸加1。&lt;br&gt;
-DL3：房间尺寸加1。场上的牌无法移动到《沙虫》所在槽位中。&lt;br&gt;
-BOSS：从额外牌堆将3张《沙虫》牌依次放在房间区任意槽位中。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DL2：房间尺寸加1。&lt;br&gt;
-DL3：房间尺寸加1。玩家的手牌只能被打出。&lt;br&gt;
-BOSS：从额外牌堆将5张《封印手指》牌洗入主牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>迷雾森林</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DL2：房间尺寸加1。&lt;br&gt;
-DL3：房间尺寸加1。重整时，房间区中央的牌保持背面向上发出。&lt;br&gt;
-BOSS：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DL2：房间尺寸加1。&lt;br&gt;
-DL3：房间尺寸加1。遗物牌使用后横置，且不会在回合结束时被复位。&lt;br&gt;
-BOSS：从额外牌堆将1张《收藏家》牌洗入主牌堆。</t>
+    <t>DL2：房间尺寸加1，手牌基数加1。墓地中的牌不受玩家控制的牌的效果影响。&lt;br&gt;
+DL3：房间尺寸加1，手牌基数加1。首次重整后，从额外牌堆将1张《命匣》牌洗入主牌堆。每次重整后，从额外牌堆将《巫妖》牌放在房间区任意槽位中。&lt;br&gt;
+胜利条件：《巫妖》牌进入墓地。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1，手牌基数加1。遗物牌使用后横置，且不会在回合结束时被复位。&lt;br&gt;
+DL3：房间尺寸加1，手牌基数加1。首次重整后，从额外牌堆将1张《收藏家》牌洗入主牌堆。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1，手牌基数加1。玩家的手牌只能被打出。&lt;br&gt;
+DL3：房间尺寸加1，手牌基数加1。首次重整后，从额外牌堆将5张《封印手指》牌洗入主牌堆。&lt;br&gt;
+胜利条件：所有《封印手指》牌进入墓地。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1，手牌基数加1。每次重整时，房间区中央的牌保持背面向上发出。&lt;br&gt;
+DL3：房间尺寸加1，手牌基数加1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1，手牌基数加1。战斗中，战场外的牌无法移入战场，战场中的牌无法移出战场。&lt;br&gt;
+DL3：房间尺寸加1，手牌基数加1。首次重整后，从额外牌堆将1张《冠军》牌放在房间区任意槽位中，然后将主牌堆所有牌送墓，此过程中不触发任何送墓时效果。&lt;br&gt;
+胜利条件：《冠军》牌进入墓地。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1，手牌基数加1。场上的牌无法移动到《沙虫》所在槽位中。&lt;br&gt;
+DL3：房间尺寸加1，手牌基数加1。首次重整后，从额外牌堆将2张《沙虫》牌依次放在房间区任意槽位中。&lt;br&gt;
+胜利条件：所有《沙虫》牌进入墓地。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -471,7 +469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -479,10 +477,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -490,10 +488,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -501,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -512,12 +510,12 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -528,13 +526,13 @@
     </row>
     <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed some too complexed or restricted item cards. Added Mead card. Renamed Lawyer Badge card to Concave Mirror and changed its effect a bit. Buffed the effect of Sphynx Salt Injector making it reveal one of all decks instead of main deck. Modified the effect of Mini Factory card and Alert Bot card. Changed the description of Mine card making it less ambiguous. Changed the rank of Miner Bot card to 2. Buffed the effect of Campfire card to cost 1 less time for each of its effect. Changed the effect of Goo card to add the rank of a nearby monster card instead of slime card. Nerfed Champion card, it does not deal damage if on the turn it's defeated.
</commit_message>
<xml_diff>
--- a/sheet/ChallengeCardData.xlsx
+++ b/sheet/ChallengeCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E15CDEA-AFE6-48AC-AE22-A30A2580B04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A237E1F9-81BB-4C0D-9A43-5CDCE8DBCFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,11 +88,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DL2：房间尺寸加1，手牌基数加1。遗物牌使用后横置，且不会在回合结束时被复位。&lt;br&gt;
-DL3：房间尺寸加1，手牌基数加1。首次重整后，从额外牌堆将1张《收藏家》牌洗入主牌堆。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DL2：房间尺寸加1，手牌基数加1。玩家的手牌只能被打出。&lt;br&gt;
 DL3：房间尺寸加1，手牌基数加1。首次重整后，从额外牌堆将5张《封印手指》牌洗入主牌堆。&lt;br&gt;
 胜利条件：所有《封印手指》牌进入墓地。</t>
@@ -113,6 +108,12 @@
     <t>DL2：房间尺寸加1，手牌基数加1。场上的牌无法移动到《沙虫》所在槽位中。&lt;br&gt;
 DL3：房间尺寸加1，手牌基数加1。首次重整后，从额外牌堆将2张《沙虫》牌依次放在房间区任意槽位中。&lt;br&gt;
 胜利条件：所有《沙虫》牌进入墓地。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL2：房间尺寸加1，手牌基数加1。遗物牌使用后横置，且不会在回合结束时被复位。&lt;br&gt;
+DL3：房间尺寸加1，手牌基数加1。首次重整后，从额外牌堆将1张《收藏家》牌洗入主牌堆。&lt;br&gt;
+胜利条件：《收藏家》牌进入墓地。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -443,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -488,10 +489,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -499,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
@@ -510,7 +511,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="57" x14ac:dyDescent="0.2">
@@ -521,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
@@ -532,7 +533,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>